<commit_message>
📊 Atualização do histórico de itens críticos - 05/08/2025 - 2 críticos de 4 itens
</commit_message>
<xml_diff>
--- a/historico_criticos.xlsx
+++ b/historico_criticos.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -458,89 +458,29 @@
           <t>Items_Criticos</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Detalhes_Criticos</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>45860</v>
+        <v>45874</v>
       </c>
       <c r="B2" t="n">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="C2" t="n">
-        <v>2582</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" s="2" t="n">
-        <v>45861</v>
-      </c>
-      <c r="B3" t="n">
-        <v>3</v>
-      </c>
-      <c r="C3" t="n">
-        <v>2582</v>
-      </c>
-      <c r="D3" t="n">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" s="2" t="n">
-        <v>45862</v>
-      </c>
-      <c r="B4" t="n">
-        <v>2.672347017815647</v>
-      </c>
-      <c r="C4" t="n">
-        <v>2582</v>
-      </c>
-      <c r="D4" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="n">
-        <v>45862</v>
-      </c>
-      <c r="B5" t="n">
-        <v>2.672347017815647</v>
-      </c>
-      <c r="C5" t="n">
-        <v>2582</v>
-      </c>
-      <c r="D5" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="2" t="n">
-        <v>45863</v>
-      </c>
-      <c r="B6" t="n">
-        <v>2.672347017815647</v>
-      </c>
-      <c r="C6" t="n">
-        <v>2582</v>
-      </c>
-      <c r="D6" t="n">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="2" t="n">
-        <v>45874</v>
-      </c>
-      <c r="B7" t="n">
-        <v>2.672347017815647</v>
-      </c>
-      <c r="C7" t="n">
-        <v>2582</v>
-      </c>
-      <c r="D7" t="n">
-        <v>69</v>
+        <v>2</v>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Material A: Crítico | Material C: Crítico</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
📊 Atualização do histórico de itens críticos - 05/08/2025 - 69 críticos de 2582 itens
</commit_message>
<xml_diff>
--- a/historico_criticos.xlsx
+++ b/historico_criticos.xlsx
@@ -469,17 +469,17 @@
         <v>45874</v>
       </c>
       <c r="B2" t="n">
-        <v>50</v>
+        <v>2.672347017815647</v>
       </c>
       <c r="C2" t="n">
-        <v>4</v>
+        <v>2582</v>
       </c>
       <c r="D2" t="n">
-        <v>2</v>
+        <v>69</v>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Material A: Crítico | Material C: Crítico</t>
+          <t>SA000009816: CRÍTICO | SC000006391: CRÍTICO | SC000006428: CRÍTICO | SC000007155: CRÍTICO | SC000007164: CRÍTICO | SC000007466: CRÍTICO | SC000007468: CRÍTICO | SC000007486: CRÍTICO | SC000032022: CRÍTICO | SC000068958: CRÍTICO</t>
         </is>
       </c>
     </row>

</xml_diff>